<commit_message>
tidyverse code with boxplot
tidyverse code with boxplot，full paper with highlight
</commit_message>
<xml_diff>
--- a/divorce.xlsx
+++ b/divorce.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Documents\GitHub\DSL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECDAC0F4-057A-400B-8FC9-51E172F27DFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5C39CB3-0C29-411B-98C7-26D3B0217614}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="21806" windowHeight="13886" xr2:uid="{C24F253F-C278-4712-AB48-1F1540FA4279}"/>
   </bookViews>
@@ -1158,8 +1158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD55A8B5-0F9F-4BE8-B0F9-3DEF5D70A426}">
   <dimension ref="A1:BC171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AK1" workbookViewId="0">
-      <selection activeCell="BD12" sqref="BD12"/>
+    <sheetView tabSelected="1" topLeftCell="AL140" workbookViewId="0">
+      <selection activeCell="AL168" sqref="AL168:BC171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>

</xml_diff>